<commit_message>
support: unity6 add: Export Static Value. improvement: Declaration of [SUBCLASS] is no longer needed.
</commit_message>
<xml_diff>
--- a/Assets/SampleData.xlsx
+++ b/Assets/SampleData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\client\github\XlsToJson\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCBA4C2-3752-4093-A4FD-A15F67281C5E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1502BF72-7ADC-44CD-AFA4-72A22E93C699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2496" yWindow="2712" windowWidth="34560" windowHeight="18684" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18996" yWindow="4764" windowWidth="27180" windowHeight="18600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Character" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="76">
   <si>
     <t/>
   </si>
@@ -138,175 +138,195 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>[SUBCLASS]</t>
-    <phoneticPr fontId="1"/>
+    <t>[CONST]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ALPHA_DEFAULT</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ALPHA_ZERO</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>BG_MORNING</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>bg01A</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>BG_NOON</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>BG_NIGHT</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>bg01B</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>bg01C</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Stage.BG_MORNING</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Stage.BG_NOON</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Stage.BG_NIGHT</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Profile01A</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Profile01B</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Profile01C</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Brightness</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>enum:AMPM</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>AM</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PM</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>AMPM</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>AM or PM</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>StageTime</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>StageTime</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>enum:StageTime</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Morning</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Noon</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Night</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>BG_MORNING = "bg01A"</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>SubClass.Child.Member0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>FriendName List</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Sex</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Unit(meter)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Number</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Light</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PPS Profile</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[ID:required]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SubClass2.Text</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SubClass2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>stage2-1</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>stage1-1</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>stage1-2</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>stage1-3</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>SubClass</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Child</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>[CONST]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ALPHA_DEFAULT</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ALPHA_ZERO</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>BG_MORNING</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>bg01A</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>BG_NOON</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>BG_NIGHT</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>bg01B</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>bg01C</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Stage.BG_MORNING</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Stage.BG_NOON</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Stage.BG_NIGHT</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Profile01A</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Profile01B</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Profile01C</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Brightness</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>enum:AMPM</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>AM</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>PM</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>AMPM</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>AM or PM</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>StageTime</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>StageTime</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>enum:StageTime</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Morning</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Noon</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Night</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>BG_MORNING = "bg01A"</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>SubClass.Child.Member0</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Name</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>FriendName List</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Sex</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Unit(meter)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Number</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Light</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>PPS Profile</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Name</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>[ID:required]</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>SubClass - Child</t>
+    <phoneticPr fontId="2"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -347,6 +367,13 @@
       <family val="3"/>
       <charset val="128"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="メイリオ"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -357,13 +384,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.59999389629810485"/>
+        <fgColor theme="3" tint="0.79985961485641044"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79985961485641044"/>
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -386,28 +413,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1084,189 +1111,186 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="13.296875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.796875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.796875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.8984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.296875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.296875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="8.796875" style="2"/>
+    <col min="1" max="1" width="13.296875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.8984375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.296875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.296875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="A1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>64</v>
+      <c r="G1" s="7" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="4"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="6"/>
+      <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="7">
+      <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="1">
         <v>1.81999999284744</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="7">
+      <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="1">
         <v>2</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="1">
         <v>1.6000000238418599</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="7">
+      <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="1">
         <v>3</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="1">
         <v>1.5</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="7"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="6"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="8"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="8"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="8"/>
@@ -1281,255 +1305,246 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="18.796875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.59765625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.3984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.296875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="20.3984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="24.8984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="23.5" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="16384" width="8.796875" style="2"/>
+    <col min="1" max="1" width="18.796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.59765625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.3984375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.296875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="20.3984375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="24.8984375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="23.5" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.3984375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:11">
+      <c r="A1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="J1" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="K1" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="K2" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="G3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="5"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="5"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="5"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="5"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="5"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="5">
         <v>0</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="5" t="s">
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7" s="8"/>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" s="8"/>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="1"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="1"/>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="1"/>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="3" t="s">
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="6" t="s">
+      <c r="B23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="6">
-        <v>1</v>
-      </c>
-      <c r="C22" s="8"/>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="6" t="s">
+      <c r="C23" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="7"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="6">
-        <v>0</v>
-      </c>
-      <c r="C23" s="8"/>
+      <c r="B24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="6" t="s">
+      <c r="A25" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D27" s="8"/>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="6" t="s">
+      <c r="B25" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>
@@ -1540,183 +1555,199 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="3.59765625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.3984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.59765625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.296875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.296875" style="2" customWidth="1"/>
-    <col min="7" max="8" width="20.3984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="24.8984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="6.8984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="16384" width="8.796875" style="2"/>
+    <col min="1" max="1" width="3.59765625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.3984375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.59765625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.296875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.296875" style="1" customWidth="1"/>
+    <col min="7" max="8" width="20.3984375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="24.8984375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.3984375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="6.8984375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:11">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>3</v>
+      </c>
+      <c r="I3" s="1">
+        <v>6</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="F4" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="5" t="s">
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>4</v>
+      </c>
+      <c r="I4" s="1">
         <v>7</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="J4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" s="1">
+        <v>2</v>
+      </c>
+      <c r="H5" s="1">
+        <v>5</v>
+      </c>
+      <c r="I5" s="1">
         <v>8</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G3" s="2">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2">
-        <v>3</v>
-      </c>
-      <c r="I3" s="2">
-        <v>6</v>
-      </c>
-      <c r="J3" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="2">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G4" s="2">
-        <v>1</v>
-      </c>
-      <c r="H4" s="2">
-        <v>4</v>
-      </c>
-      <c r="I4" s="2">
-        <v>7</v>
-      </c>
-      <c r="J4" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="2">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="G5" s="2">
-        <v>2</v>
-      </c>
-      <c r="H5" s="2">
-        <v>5</v>
-      </c>
-      <c r="I5" s="2">
-        <v>8</v>
-      </c>
-      <c r="J5" s="2">
+      <c r="J5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K5" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1728,119 +1759,129 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="3.5" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.3984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.5" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.5" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.8984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="19.09765625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="23.5" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="6.296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.796875" style="2"/>
+    <col min="1" max="1" width="3.5" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.3984375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.5" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.5" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.8984375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="19.09765625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="23.5" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.3984375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="6.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:11">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="J1" s="3" t="s">
+      <c r="I1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:11">
+      <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="E2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="2">
+    <row r="3" spans="1:11">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="2" t="b">
+      <c r="B3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>1</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>1</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <v>0</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="1">
         <v>3</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="1">
         <v>6</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K3" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>